<commit_message>
bug fixing and re uploading
</commit_message>
<xml_diff>
--- a/Data/AgingMatured.xlsx
+++ b/Data/AgingMatured.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="387">
   <si>
     <t>Cust ID</t>
   </si>
@@ -46,1009 +46,1135 @@
     <t>43061104782</t>
   </si>
   <si>
-    <t>43061109178</t>
-  </si>
-  <si>
-    <t>4301901209</t>
+    <t>4201118395</t>
+  </si>
+  <si>
+    <t>4201118043</t>
+  </si>
+  <si>
+    <t>90000006012</t>
+  </si>
+  <si>
+    <t>43061101800</t>
+  </si>
+  <si>
+    <t>90000008724</t>
+  </si>
+  <si>
+    <t>43061104555</t>
+  </si>
+  <si>
+    <t>43061109604</t>
+  </si>
+  <si>
+    <t>90000047000</t>
+  </si>
+  <si>
+    <t>43061104892</t>
+  </si>
+  <si>
+    <t>43061110163</t>
+  </si>
+  <si>
+    <t>90000045498</t>
+  </si>
+  <si>
+    <t>90000003726</t>
+  </si>
+  <si>
+    <t>43061100760</t>
+  </si>
+  <si>
+    <t>90000029247</t>
+  </si>
+  <si>
+    <t>90000044336</t>
+  </si>
+  <si>
+    <t>43061101908</t>
+  </si>
+  <si>
+    <t>4201117970</t>
+  </si>
+  <si>
+    <t>90000030489</t>
+  </si>
+  <si>
+    <t>43061000918</t>
+  </si>
+  <si>
+    <t>90000041601</t>
+  </si>
+  <si>
+    <t>43061100261</t>
+  </si>
+  <si>
+    <t>90000019175</t>
   </si>
   <si>
     <t>43061100638</t>
   </si>
   <si>
+    <t>43061109928</t>
+  </si>
+  <si>
+    <t>43061109445</t>
+  </si>
+  <si>
+    <t>90000011704</t>
+  </si>
+  <si>
+    <t>90000027006</t>
+  </si>
+  <si>
     <t>90000042935</t>
   </si>
   <si>
-    <t>90000029247</t>
-  </si>
-  <si>
-    <t>43061101800</t>
-  </si>
-  <si>
-    <t>4201118395</t>
-  </si>
-  <si>
-    <t>43061109928</t>
-  </si>
-  <si>
-    <t>90000011704</t>
-  </si>
-  <si>
-    <t>43061109625</t>
+    <t>43061101410</t>
+  </si>
+  <si>
+    <t>43061104704</t>
+  </si>
+  <si>
+    <t>43061101018</t>
+  </si>
+  <si>
+    <t>90000030491</t>
+  </si>
+  <si>
+    <t>90000033264</t>
+  </si>
+  <si>
+    <t>43061101046</t>
+  </si>
+  <si>
+    <t>90000040569</t>
+  </si>
+  <si>
+    <t>43061109315</t>
+  </si>
+  <si>
+    <t>43061000939</t>
+  </si>
+  <si>
+    <t>4306110224</t>
+  </si>
+  <si>
+    <t>43061101289</t>
+  </si>
+  <si>
+    <t>43061100434</t>
+  </si>
+  <si>
+    <t>90000041133</t>
+  </si>
+  <si>
+    <t>90000020550</t>
+  </si>
+  <si>
+    <t>90000049228</t>
+  </si>
+  <si>
+    <t>43061109296</t>
+  </si>
+  <si>
+    <t>43061000925</t>
+  </si>
+  <si>
+    <t>43061000683</t>
+  </si>
+  <si>
+    <t>43061109109</t>
+  </si>
+  <si>
+    <t>43061100715</t>
+  </si>
+  <si>
+    <t>43061109378</t>
+  </si>
+  <si>
+    <t>90000034068</t>
+  </si>
+  <si>
+    <t>43061000942</t>
+  </si>
+  <si>
+    <t>43061100998</t>
+  </si>
+  <si>
+    <t>43061110086</t>
+  </si>
+  <si>
+    <t>90000030738</t>
+  </si>
+  <si>
+    <t>43061109822</t>
+  </si>
+  <si>
+    <t>90000031237</t>
+  </si>
+  <si>
+    <t>43061100743</t>
+  </si>
+  <si>
+    <t>43061193121</t>
+  </si>
+  <si>
+    <t>43061000146</t>
+  </si>
+  <si>
+    <t>43061109987</t>
+  </si>
+  <si>
+    <t>90000022235</t>
+  </si>
+  <si>
+    <t>90000023957</t>
+  </si>
+  <si>
+    <t>90000027463</t>
   </si>
   <si>
     <t>90000022393</t>
   </si>
   <si>
-    <t>4201117970</t>
-  </si>
-  <si>
-    <t>43061100760</t>
-  </si>
-  <si>
-    <t>90000030491</t>
-  </si>
-  <si>
-    <t>90000045498</t>
-  </si>
-  <si>
-    <t>43061109604</t>
-  </si>
-  <si>
-    <t>43061100261</t>
-  </si>
-  <si>
-    <t>90000041601</t>
-  </si>
-  <si>
-    <t>90000003726</t>
-  </si>
-  <si>
-    <t>43061000146</t>
-  </si>
-  <si>
-    <t>43061100743</t>
-  </si>
-  <si>
-    <t>43061100434</t>
-  </si>
-  <si>
-    <t>43061000991</t>
-  </si>
-  <si>
-    <t>43061101018</t>
-  </si>
-  <si>
-    <t>43061109445</t>
-  </si>
-  <si>
-    <t>43061101289</t>
-  </si>
-  <si>
-    <t>43061101046</t>
-  </si>
-  <si>
-    <t>90000019175</t>
-  </si>
-  <si>
-    <t>90000033264</t>
-  </si>
-  <si>
-    <t>43061100351</t>
-  </si>
-  <si>
-    <t>90000027006</t>
-  </si>
-  <si>
-    <t>90000044336</t>
-  </si>
-  <si>
-    <t>43061101144</t>
-  </si>
-  <si>
-    <t>43061101077</t>
-  </si>
-  <si>
-    <t>43061110093</t>
-  </si>
-  <si>
-    <t>43061104555</t>
-  </si>
-  <si>
-    <t>90000020550</t>
-  </si>
-  <si>
-    <t>43061110163</t>
-  </si>
-  <si>
-    <t>90000023957</t>
-  </si>
-  <si>
-    <t>90000040569</t>
-  </si>
-  <si>
-    <t>90000027463</t>
-  </si>
-  <si>
-    <t>43061109315</t>
-  </si>
-  <si>
-    <t>43061101908</t>
-  </si>
-  <si>
-    <t>43061101504</t>
-  </si>
-  <si>
-    <t>43061110099</t>
-  </si>
-  <si>
-    <t>43061109423</t>
-  </si>
-  <si>
-    <t>43061000192</t>
-  </si>
-  <si>
-    <t>43061000683</t>
-  </si>
-  <si>
-    <t>43061109618</t>
-  </si>
-  <si>
-    <t>43061101378</t>
-  </si>
-  <si>
-    <t>43061101392</t>
-  </si>
-  <si>
-    <t>43061104122</t>
-  </si>
-  <si>
-    <t>43061104682</t>
-  </si>
-  <si>
-    <t>90000030489</t>
+    <t>43061109175</t>
+  </si>
+  <si>
+    <t>43061104345</t>
+  </si>
+  <si>
+    <t>43061100438</t>
+  </si>
+  <si>
+    <t>90000026236</t>
+  </si>
+  <si>
+    <t>43061100275</t>
+  </si>
+  <si>
+    <t>90000045908</t>
+  </si>
+  <si>
+    <t>43061109670</t>
+  </si>
+  <si>
+    <t>90000003418</t>
   </si>
   <si>
     <t>90000012105</t>
   </si>
   <si>
-    <t>43061109175</t>
-  </si>
-  <si>
     <t>43061109826</t>
   </si>
   <si>
-    <t>43061000916</t>
+    <t>43061100422</t>
   </si>
   <si>
     <t>43061109713</t>
   </si>
   <si>
-    <t>43061104719</t>
-  </si>
-  <si>
-    <t>90000045908</t>
-  </si>
-  <si>
-    <t>43061100210</t>
-  </si>
-  <si>
-    <t>43061100932</t>
-  </si>
-  <si>
-    <t>43061109378</t>
-  </si>
-  <si>
-    <t>43061001723</t>
-  </si>
-  <si>
-    <t>43061101262</t>
-  </si>
-  <si>
-    <t>43061101084</t>
-  </si>
-  <si>
-    <t>43061101459</t>
-  </si>
-  <si>
-    <t>4301901720</t>
-  </si>
-  <si>
-    <t>430190938</t>
-  </si>
-  <si>
-    <t>43061101349</t>
-  </si>
-  <si>
     <t>Niramoy Pharmacy</t>
   </si>
   <si>
-    <t>Jesmin Parmacy</t>
-  </si>
-  <si>
-    <t>Ruma Pharmacy</t>
+    <t>Molla Pharmacy</t>
+  </si>
+  <si>
+    <t>The Medical Center</t>
+  </si>
+  <si>
+    <t>Al Bab Medical Hall</t>
+  </si>
+  <si>
+    <t>Renasase Med Centre</t>
+  </si>
+  <si>
+    <t>Shefa Clinic</t>
+  </si>
+  <si>
+    <t>Opu Pharmacy</t>
+  </si>
+  <si>
+    <t>Dr Eanur</t>
+  </si>
+  <si>
+    <t>Doctor Bari Pharmacy</t>
+  </si>
+  <si>
+    <t>Dr Belal Med Hall</t>
+  </si>
+  <si>
+    <t>Salam Medicine Corner</t>
+  </si>
+  <si>
+    <t>Abdullah Pharmacy</t>
+  </si>
+  <si>
+    <t>M S Selina Drug House</t>
+  </si>
+  <si>
+    <t>Kamal Pharmacy</t>
+  </si>
+  <si>
+    <t>Amena Medical Stor</t>
+  </si>
+  <si>
+    <t>Maa Fatema Medical Hall</t>
+  </si>
+  <si>
+    <t>Ashif Pharmacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bishwa Nath Medical </t>
+  </si>
+  <si>
+    <t>Emon Pharmacy</t>
+  </si>
+  <si>
+    <t>Orient Pharmacy</t>
+  </si>
+  <si>
+    <t>Ritu Pharmacy</t>
+  </si>
+  <si>
+    <t>Anower Medical Hall</t>
+  </si>
+  <si>
+    <t>Nipa Pharmacy</t>
   </si>
   <si>
     <t>Janasheba Pharmacy</t>
   </si>
   <si>
+    <t>Sarder Medical</t>
+  </si>
+  <si>
+    <t>Nahar Pharmacy</t>
+  </si>
+  <si>
+    <t>Chitholia Medical Store</t>
+  </si>
+  <si>
+    <t>Medicine Corner</t>
+  </si>
+  <si>
     <t>Islamia Pharmacy</t>
   </si>
   <si>
-    <t>Amena Medical Stor</t>
-  </si>
-  <si>
-    <t>Renasase Med Centre</t>
-  </si>
-  <si>
-    <t>Molla Pharmacy</t>
-  </si>
-  <si>
-    <t>Sarder Medical</t>
-  </si>
-  <si>
-    <t>Chitholia Medical Store</t>
-  </si>
-  <si>
-    <t>Siddik Pharmacy</t>
+    <t>Arko Pharmacy</t>
+  </si>
+  <si>
+    <t>Joti Pharmacy</t>
+  </si>
+  <si>
+    <t>Samsul Alam PHARMACY</t>
+  </si>
+  <si>
+    <t>Papri Pharmacy</t>
+  </si>
+  <si>
+    <t>Biswas Pharmacy</t>
+  </si>
+  <si>
+    <t>Zaman Pharmacy</t>
+  </si>
+  <si>
+    <t>Dr Dablu</t>
+  </si>
+  <si>
+    <t>Bulbul Pharmacy</t>
+  </si>
+  <si>
+    <t>Tultul Medicare</t>
+  </si>
+  <si>
+    <t>Nafiz Pharmacy</t>
+  </si>
+  <si>
+    <t>Remidy Pharmacy</t>
+  </si>
+  <si>
+    <t>M S kushtia Optical</t>
+  </si>
+  <si>
+    <t>Habib Medical Hall</t>
+  </si>
+  <si>
+    <t>United Clinic</t>
+  </si>
+  <si>
+    <t>Mahbub Pharmacy</t>
+  </si>
+  <si>
+    <t>Romesh Clinic</t>
+  </si>
+  <si>
+    <t>Royal Pharmacy</t>
+  </si>
+  <si>
+    <t>Nipu Pharmacy</t>
+  </si>
+  <si>
+    <t>Bangladesh Pharmacy</t>
+  </si>
+  <si>
+    <t>Khalid And Abir Pharmacy</t>
+  </si>
+  <si>
+    <t>Jim Pharmacy</t>
+  </si>
+  <si>
+    <t>Jibon Pharmacy</t>
+  </si>
+  <si>
+    <t>Tohid Pharmacy</t>
+  </si>
+  <si>
+    <t>Jaci Pharmacy</t>
+  </si>
+  <si>
+    <t>Biozid Pharmacy</t>
+  </si>
+  <si>
+    <t>Bismillah Clinic</t>
+  </si>
+  <si>
+    <t>Uposhom Narsing Home</t>
+  </si>
+  <si>
+    <t>Maha Maya Pharmacy</t>
+  </si>
+  <si>
+    <t>Lokman Clinic</t>
+  </si>
+  <si>
+    <t>Medinova Center</t>
+  </si>
+  <si>
+    <t>Ster Pharmacy</t>
+  </si>
+  <si>
+    <t>Anisha Pharmacy</t>
+  </si>
+  <si>
+    <t>Bhai Bhai Pharmacy</t>
+  </si>
+  <si>
+    <t>Maya Medical Hall</t>
   </si>
   <si>
     <t>Rashida Medical Hall</t>
   </si>
   <si>
-    <t xml:space="preserve">Bishwa Nath Medical </t>
-  </si>
-  <si>
-    <t>Kamal Pharmacy</t>
-  </si>
-  <si>
-    <t>Papri Pharmacy</t>
-  </si>
-  <si>
-    <t>Abdullah Pharmacy</t>
-  </si>
-  <si>
-    <t>Dr Eanur</t>
-  </si>
-  <si>
-    <t>Anower Medical Hall</t>
-  </si>
-  <si>
-    <t>Ritu Pharmacy</t>
-  </si>
-  <si>
-    <t>M S Selina Drug House</t>
-  </si>
-  <si>
-    <t>Medinova Center</t>
-  </si>
-  <si>
-    <t>Maha Maya Pharmacy</t>
-  </si>
-  <si>
-    <t>Remidy Pharmacy</t>
-  </si>
-  <si>
-    <t>Ahmed Pharmacy</t>
-  </si>
-  <si>
-    <t>Samsul Alam PHARMACY</t>
-  </si>
-  <si>
-    <t>Nahar Pharmacy</t>
-  </si>
-  <si>
-    <t>Nafiz Pharmacy</t>
-  </si>
-  <si>
-    <t>Zaman Pharmacy</t>
-  </si>
-  <si>
-    <t>Nipa Pharmacy</t>
-  </si>
-  <si>
-    <t>Biswas Pharmacy</t>
-  </si>
-  <si>
-    <t>Zaved Pharmacy</t>
-  </si>
-  <si>
-    <t>Medicine Corner</t>
-  </si>
-  <si>
-    <t>Maa Fatema Medical Hall</t>
-  </si>
-  <si>
-    <t>Mahabub Pharmacy</t>
-  </si>
-  <si>
-    <t>Jannati Pharmacy</t>
-  </si>
-  <si>
-    <t>Sarker Pharmacy</t>
-  </si>
-  <si>
-    <t>Opu Pharmacy</t>
-  </si>
-  <si>
-    <t>Habib Medical Hall</t>
-  </si>
-  <si>
-    <t>Salam Medicine Corner</t>
-  </si>
-  <si>
-    <t>Bhai Bhai Pharmacy</t>
-  </si>
-  <si>
-    <t>Maya Medical Hall</t>
-  </si>
-  <si>
-    <t>Dr Dablu</t>
-  </si>
-  <si>
-    <t>Ashif Pharmacy</t>
-  </si>
-  <si>
-    <t>Ali Pharmacy</t>
-  </si>
-  <si>
-    <t>Sithi Drug House</t>
-  </si>
-  <si>
-    <t>Kushtia Surgical</t>
-  </si>
-  <si>
-    <t>Islami Hospital</t>
-  </si>
-  <si>
-    <t>Royal Pharmacy</t>
-  </si>
-  <si>
-    <t>Ashraful Pharmacy</t>
-  </si>
-  <si>
-    <t>H Pharmacy</t>
-  </si>
-  <si>
-    <t>Uttom Drug House</t>
-  </si>
-  <si>
-    <t>Maa Medical Hall</t>
-  </si>
-  <si>
-    <t>Sonar Bangla Pharmacy</t>
-  </si>
-  <si>
-    <t>Emon Pharmacy</t>
+    <t>Joy Pharmacy</t>
+  </si>
+  <si>
+    <t>Seraton Medical Hall</t>
+  </si>
+  <si>
+    <t>Tuhin Pharmacy</t>
+  </si>
+  <si>
+    <t>Kazi Pharmacy</t>
+  </si>
+  <si>
+    <t>Dr Alauddin</t>
+  </si>
+  <si>
+    <t>Gangni Sono Diagnostic&amp;Clinic</t>
+  </si>
+  <si>
+    <t>Salam Pharmacy</t>
+  </si>
+  <si>
+    <t>Bismillah Pharmacy &amp; Chikitsha</t>
   </si>
   <si>
     <t>Sazu Drug House</t>
   </si>
   <si>
-    <t>Joy Pharmacy</t>
-  </si>
-  <si>
     <t>M S Nupur Pharmacy</t>
   </si>
   <si>
-    <t>Mithun Drug House</t>
+    <t>Bajlo Medical Holl</t>
   </si>
   <si>
     <t>Life Care Pharmacy</t>
   </si>
   <si>
-    <t>Limon Drug House</t>
-  </si>
-  <si>
-    <t>Gangni Sono Diagnostic&amp;Clinic</t>
-  </si>
-  <si>
-    <t>Health Care</t>
-  </si>
-  <si>
-    <t>Sumaya Medical Hall</t>
-  </si>
-  <si>
-    <t>Khalid And Abir Pharmacy</t>
-  </si>
-  <si>
-    <t>Selim Pharmacy</t>
-  </si>
-  <si>
-    <t>Star Pharmacy</t>
-  </si>
-  <si>
-    <t>Mim Pharmacy</t>
-  </si>
-  <si>
-    <t>Janoni Pharmacy</t>
-  </si>
-  <si>
-    <t>Adhikari Pharmacy</t>
-  </si>
-  <si>
-    <t>Khandokar Pharmacy</t>
-  </si>
-  <si>
-    <t>Synthia Care Clinic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chand Market Gorahmara Shimultala                           </t>
   </si>
   <si>
-    <t xml:space="preserve">Jhawdia Bazar Bittipara                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polish Line Magura                                          </t>
+    <t xml:space="preserve">Pangsha Bzaer Rajbari                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Fornt of Upzela Pangsha                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamalpur,Shampur,Daulotpur                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khalishakundi Mirpur                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ershadpur, Alamdanga                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorshona Bus Stand Dorshona                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sahapur Andulbaria Jibonnagar                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badargonj Bazar.Choudanga                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allardorga Bazar ,Daulotpur                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurulgachi Bazar Dorshona Chuadanga                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halt Station Dorsona                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fultola Chowrhas More                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goal Para Bazar Jhenaidha                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allardarga Bazar.Doulatpur Kushtia.                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nandolaur.Kumarkhali.Kushtia                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Road Kushtia                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatulia Bazar Baliakandi                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raghunatpur.Chuadanga                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circit House Meherpur                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdalpur Bazar,Kushtia.                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andol Baria Jibonnagar Chuadanga                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuchiamara Bazar                                            </t>
   </si>
   <si>
     <t xml:space="preserve">Amerchara more Parbotipur Horinakundo                       </t>
   </si>
   <si>
+    <t xml:space="preserve">Baliasisa Sherpur Mirpur                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital gate Meherpur meherpur Meherpur                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chitholia Bazar, Mirpur                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuchiamora Bazar,Bheramara                                  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Maspara Bazar,Pangsha.Rajbari                               </t>
   </si>
   <si>
-    <t xml:space="preserve">Allardarga Bazar.Doulatpur Kushtia.                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khalishakundi Mirpur                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pangsha Bzaer Rajbari                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baliasisa Sherpur Mirpur                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chitholia Bazar, Mirpur                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shauta Bridge Badh Bazar Panti Kushtia                      </t>
+    <t xml:space="preserve">Sastripur Vadalia Kushtia                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vadalia Bazar Kushtia                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hemayatpur  Bazar Gangni Meherpur                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roghunatpur.Chuadanga.                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toltoli ParaDaulatpur Kushtia.                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bashbaria Bazar Gangni Meherpur                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Railway Gate.Haksha Bazar.Mirpur.Kushtia.                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boliarpur Bazar Baradi Meherpur                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gangni Bazar Meherpur                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kedergonj Bazar Chuadanga                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godawan More,Main Road Bheramara                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khaskorra Bazar Sarojgonj                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N S Road Toffazzol Health care                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KederGonj Bazar, Mujibnagar                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Road Choudanga                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patika Bari Phorada Kushtia                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mollik Para Meherpur                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">School Market Shoilokupa                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hatfajilpur Bazar Shoilokupa                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Number Panir Tank Adarsha Para Jhenaidha              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Gate Horinakundu Jhenidah                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haravanga Possimpara Poscimpara                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bamundi Bazar                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dariapur Bazar Mujibnagar                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chitulia Mirpur Kushtia                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R S Market.Kushtia                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kanabil More Jugia Kushtia                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Road.Choudanga.                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tikari More Jhenaidha                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">College Para Alamdanga                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Court Road Chuadanga                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazi More Alamdanga                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Road,Alamdanga                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Komorpur,Mujibnagar                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osmanpur,Khoksha                                            </t>
   </si>
   <si>
     <t xml:space="preserve">Polash Market Rajbari Road Boharpur Bazar Rajbari           </t>
   </si>
   <si>
-    <t xml:space="preserve">Tatulia Bazar Baliakandi                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goal Para Bazar Jhenaidha                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roghunatpur.Chuadanga.                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halt Station Dorsona                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sahapur Andulbaria Jibonnagar                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andol Baria Jibonnagar Chuadanga                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abdalpur Bazar,Kushtia.                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fultola Chowrhas More                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Court Road Chuadanga                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tikari More Jhenaidha                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khaskorra Bazar Sarojgonj                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Razzaque Super Market Kushtia                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hemayatpur  Bazar Gangni Meherpur                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital gate Meherpur meherpur Meherpur                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godawan More,Main Road Bheramara                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bashbaria Bazar Gangni Meherpur                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kuchiamara Bazar                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toltoli ParaDaulatpur Kushtia.                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andulbaria Bazar Darshona                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kuchiamora Bazar,Bheramara                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nandolaur.Kumarkhali.Kushtia                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potherhat Bazar Sattajitpur                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gazir More Mohammad Pur                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jogoti Rail Bazar Jogoti Kushtia                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dorshona Bus Stand Dorshona                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KederGonj Bazar, Mujibnagar                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kurulgachi Bazar Dorshona Chuadanga                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Komorpur,Mujibnagar                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Railway Gate.Haksha Bazar.Mirpur.Kushtia.                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osmanpur,Khoksha                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boliarpur Bazar Baradi Meherpur                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Road Kushtia                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joy Bangla Bazar Panti                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Singra Bazar Arpara Magura                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kataikhana More Kushtia                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Road Chuadanga                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">School Market Shoilokupa                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patikabari Halsa                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halsa Bazar Mirpur                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr Kartick Madhupur Bazar Panti                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nagra Bazar Mohammadpur Magura                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raghunatpur.Chuadanga                                       </t>
+    <t xml:space="preserve">Notun Bazar Mirpur.                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C O Rabiul Islam Razarhat More Kushtia                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badargonj Bazar Chuadanga                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damurhuda Bazar                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gurdah Bazar Jibonnagar                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Bazar Gangni Meherpur                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panti Bazar Kumarkhali                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 No. Bridge, Bheramara                                     </t>
   </si>
   <si>
     <t xml:space="preserve">Beside of Hasan Clinic Jhinaidah                            </t>
   </si>
   <si>
-    <t xml:space="preserve">Notun Bazar Mirpur.                                         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sarojgonj Bazar Chuadanga                                   </t>
   </si>
   <si>
-    <t xml:space="preserve">Kedergonj Bazar Mojibnagor                                  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Shanti Para Choudanga                                       </t>
   </si>
   <si>
-    <t xml:space="preserve">Hospital Road Chuadanga Chuadanga                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Bazar Gangni Meherpur                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawlotdiar Chuadanga                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Gate Kedargonj Meherpur                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Gate Horinakundu Jhenidah                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amla Bazar Mirpur                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kumarkhali Kushtia                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Itvata Bazar Laxmipur Laxmipur                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bunagati Bazar Magura                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thana More Daulotpur                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve">KC35                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve">KC15                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR71                                                        </t>
+    <t xml:space="preserve">KC82                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC81                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC32                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC33                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC63                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC53                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC65                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC34                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC11                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC45                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC22                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC24                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC83                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC71                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC13                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC31                                                        </t>
   </si>
   <si>
     <t xml:space="preserve">KC44                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve">KC82                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC34                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC33                                                        </t>
+    <t xml:space="preserve">KC72                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC73                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC14                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC51                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC74                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC61                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC43                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC42                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC75                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC21                                                        </t>
   </si>
   <si>
     <t xml:space="preserve">KC25                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve">KC83                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC45                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC53                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC13                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC11                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC51                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC42                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC65                                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve">KC12                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve">KC73                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC72                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC31                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC22                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR63                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC74                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC14                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC24                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR72                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC43                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC61                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR64                                                        </t>
+    <t xml:space="preserve">KC62                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC52                                                        </t>
   </si>
   <si>
     <t xml:space="preserve">KC41                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve">KC32                                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve">SKINV430-502523     </t>
   </si>
   <si>
-    <t xml:space="preserve">SKINV430-553218     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-557365     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-570783     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571314     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571506     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571362     </t>
-  </si>
-  <si>
     <t xml:space="preserve">SKINV430-571195     </t>
   </si>
   <si>
-    <t xml:space="preserve">SKINV430-571499     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571429     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-559445     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571596     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571605     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571961     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571902     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571975     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571760     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572066     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571709     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571669     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-559815     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-571756     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572369     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-560178     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572398     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572394     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-560386     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572128     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572869     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572717     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-560954     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572800     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-572884     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-560543     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-560540     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-560755     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573485     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573205     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573482     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573206     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573342     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-561228     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573272     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573196     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-561238     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-561672     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-561721     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562328     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-573993     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562287     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562064     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562047     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562374     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562503     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-575096     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562744     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562862     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563105     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563023     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562782     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562948     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563084     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563025     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562907     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-562970     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563345     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563480     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563514     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563351     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563266     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563273     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV430-563329     </t>
+    <t xml:space="preserve">SKINV430-576011     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-577547     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-577428     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-566768     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-580913     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-580688     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-581127     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-581443     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-581951     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-582184     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-582233     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-582653     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583047     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583079     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583086     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583463     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583568     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-570942     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583404     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583527     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583837     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583691     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583703     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584155     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583712     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-583696     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584517     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-572113     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-572081     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584974     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584879     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584537     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584563     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584699     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-584622     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-572472     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-572232     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-572957     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-585229     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-585407     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-585674     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-573360     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-573573     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-585472     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-585514     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-573816     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-573992     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-573985     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-586873     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-586943     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-586709     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-574612     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-587310     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-587258     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-574475     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-574932     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-587244     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-574922     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-574903     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-588040     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-588028     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-587780     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-575286     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-588179     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-575953     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-576198     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-588293     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-588531     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-576326     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-576208     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-589079     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-588913     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-576760     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-589020     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-576634     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-577140     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-577179     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-577075     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-577036     </t>
   </si>
   <si>
     <t>05 Aug 2020</t>
   </si>
   <si>
-    <t>19 Nov 2020</t>
-  </si>
-  <si>
-    <t>29 Nov 2020</t>
+    <t>03 Jan 2021</t>
+  </si>
+  <si>
+    <t>13 Jan 2021</t>
+  </si>
+  <si>
+    <t>17 Jan 2021</t>
+  </si>
+  <si>
+    <t>21 Dec 2020</t>
+  </si>
+  <si>
+    <t>25 Jan 2021</t>
+  </si>
+  <si>
+    <t>26 Jan 2021</t>
+  </si>
+  <si>
+    <t>27 Jan 2021</t>
+  </si>
+  <si>
+    <t>28 Jan 2021</t>
+  </si>
+  <si>
+    <t>29 Jan 2021</t>
+  </si>
+  <si>
+    <t>30 Jan 2021</t>
+  </si>
+  <si>
+    <t>31 Jan 2021</t>
+  </si>
+  <si>
+    <t>01 Feb 2021</t>
   </si>
   <si>
     <t>02 Jan 2021</t>
   </si>
   <si>
-    <t>03 Jan 2021</t>
-  </si>
-  <si>
-    <t>04 Dec 2020</t>
+    <t>02 Feb 2021</t>
+  </si>
+  <si>
+    <t>03 Feb 2021</t>
   </si>
   <si>
     <t>04 Jan 2021</t>
   </si>
   <si>
-    <t>05 Dec 2020</t>
+    <t>04 Feb 2021</t>
   </si>
   <si>
     <t>05 Jan 2021</t>
   </si>
   <si>
-    <t>06 Dec 2020</t>
-  </si>
-  <si>
     <t>06 Jan 2021</t>
   </si>
   <si>
-    <t>07 Dec 2020</t>
+    <t>06 Feb 2021</t>
   </si>
   <si>
     <t>07 Jan 2021</t>
   </si>
   <si>
-    <t>08 Dec 2020</t>
-  </si>
-  <si>
-    <t>09 Dec 2020</t>
-  </si>
-  <si>
-    <t>10 Dec 2020</t>
-  </si>
-  <si>
     <t>09 Jan 2021</t>
   </si>
   <si>
-    <t>11 Dec 2020</t>
+    <t>09 Feb 2021</t>
+  </si>
+  <si>
+    <t>10 Jan 2021</t>
+  </si>
+  <si>
+    <t>10 Feb 2021</t>
   </si>
   <si>
     <t>11 Jan 2021</t>
   </si>
   <si>
-    <t>12 Dec 2020</t>
-  </si>
-  <si>
-    <t>13 Dec 2020</t>
+    <t>11 Feb 2021</t>
+  </si>
+  <si>
+    <t>12 Jan 2021</t>
+  </si>
+  <si>
+    <t>12 Feb 2021</t>
+  </si>
+  <si>
+    <t>14 Jan 2021</t>
+  </si>
+  <si>
+    <t>13 Feb 2021</t>
+  </si>
+  <si>
+    <t>14 Feb 2021</t>
+  </si>
+  <si>
+    <t>15 Jan 2021</t>
+  </si>
+  <si>
+    <t>16 Jan 2021</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1461,28 +1587,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="F2" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="G2" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="H2">
         <v>30</v>
       </c>
       <c r="I2">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="J2">
-        <v>5087.96</v>
+        <v>3587.96</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1493,28 +1619,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="F3" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="G3" t="s">
-        <v>325</v>
+        <v>353</v>
       </c>
       <c r="H3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="J3">
-        <v>3380.29</v>
+        <v>3379.15</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1525,28 +1651,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="F4" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="G4" t="s">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="J4">
-        <v>6761.08</v>
+        <v>22984.02</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1557,28 +1683,28 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="F5" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="G5" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="J5">
-        <v>11874.07</v>
+        <v>29944.37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1589,28 +1715,28 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="F6" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="G6" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J6">
-        <v>50025.66</v>
+        <v>20040.05</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1621,28 +1747,28 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="F7" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="G7" t="s">
-        <v>328</v>
+        <v>356</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J7">
-        <v>30047.96</v>
+        <v>12000.73</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1653,28 +1779,28 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="G8" t="s">
-        <v>328</v>
+        <v>357</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J8">
-        <v>19879.04</v>
+        <v>19458.12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1685,28 +1811,28 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E9" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="F9" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="G9" t="s">
-        <v>328</v>
+        <v>357</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J9">
-        <v>14879.15</v>
+        <v>9839.27</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1717,28 +1843,28 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="F10" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="G10" t="s">
-        <v>328</v>
+        <v>358</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="J10">
-        <v>12027.12</v>
+        <v>34716.14</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1749,28 +1875,28 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="F11" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="G11" t="s">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J11">
-        <v>6994.36</v>
+        <v>25198.49</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1781,28 +1907,28 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="F12" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="G12" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
       <c r="H12">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J12">
-        <v>5036.26</v>
+        <v>19741.02</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1813,28 +1939,28 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="F13" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="G13" t="s">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="J13">
-        <v>20061.52</v>
+        <v>9954.200000000001</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1845,28 +1971,28 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="F14" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="G14" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J14">
-        <v>20022.54</v>
+        <v>1500.95</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1877,28 +2003,28 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E15" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="G15" t="s">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J15">
-        <v>14906.48</v>
+        <v>12761.05</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1909,28 +2035,28 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="F16" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="G16" t="s">
-        <v>330</v>
+        <v>363</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J16">
-        <v>14283.94</v>
+        <v>29871.3</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1941,28 +2067,28 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="F17" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="G17" t="s">
-        <v>330</v>
+        <v>363</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J17">
-        <v>10026.5</v>
+        <v>5139.4</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1973,28 +2099,28 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E18" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="F18" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="G18" t="s">
-        <v>330</v>
+        <v>363</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J18">
-        <v>9697.969999999999</v>
+        <v>4953.19</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2005,28 +2131,28 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F19" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="G19" t="s">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J19">
-        <v>9628.540000000001</v>
+        <v>19940.27</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2037,28 +2163,28 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F20" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="G20" t="s">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J20">
-        <v>6672.56</v>
+        <v>19541.16</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2069,28 +2195,28 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="F21" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="G21" t="s">
-        <v>330</v>
+        <v>365</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I21">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J21">
-        <v>3531.01</v>
+        <v>14914.1</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2101,28 +2227,28 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E22" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="F22" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G22" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
       <c r="H22">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J22">
-        <v>3055.69</v>
+        <v>9890.02</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2133,28 +2259,28 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E23" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="F23" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="G23" t="s">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J23">
-        <v>2711.12</v>
+        <v>9854.75</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2165,28 +2291,28 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="F24" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="G24" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J24">
-        <v>29599.91</v>
+        <v>24670.88</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2197,28 +2323,28 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="E25" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="F25" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="G25" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
       <c r="H25">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J25">
-        <v>29122.44</v>
+        <v>12211.04</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2229,28 +2355,28 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E26" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F26" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="G26" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J26">
-        <v>25122.84</v>
+        <v>12024.55</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2261,28 +2387,28 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E27" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F27" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="G27" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J27">
-        <v>10058.83</v>
+        <v>10114.4</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2293,28 +2419,28 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E28" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F28" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="G28" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
       <c r="H28">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J28">
-        <v>6000.51</v>
+        <v>7296.36</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2325,28 +2451,28 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E29" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="F29" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="G29" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J29">
-        <v>5069.6</v>
+        <v>4637.29</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2357,28 +2483,28 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F30" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="G30" t="s">
-        <v>334</v>
+        <v>367</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J30">
-        <v>23938.34</v>
+        <v>50010.13</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2389,28 +2515,28 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="E31" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="F31" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
       <c r="G31" t="s">
-        <v>334</v>
+        <v>368</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I31">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J31">
-        <v>10019.89</v>
+        <v>9776.290000000001</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2421,28 +2547,28 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F32" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="G32" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
       <c r="H32">
         <v>30</v>
       </c>
       <c r="I32">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J32">
-        <v>7106.32</v>
+        <v>424.73</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2453,28 +2579,28 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E33" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="F33" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="G33" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J33">
-        <v>6696.59</v>
+        <v>25067.7</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2485,28 +2611,28 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="E34" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F34" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="G34" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J34">
-        <v>5087.52</v>
+        <v>14684.18</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2517,28 +2643,28 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="E35" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="F35" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="G35" t="s">
-        <v>335</v>
+        <v>369</v>
       </c>
       <c r="H35">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J35">
-        <v>4965.46</v>
+        <v>10016.22</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2549,28 +2675,28 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E36" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="F36" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
       <c r="G36" t="s">
-        <v>335</v>
+        <v>369</v>
       </c>
       <c r="H36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J36">
-        <v>3022.63</v>
+        <v>5199.22</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2581,28 +2707,28 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E37" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="F37" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
       <c r="G37" t="s">
-        <v>335</v>
+        <v>369</v>
       </c>
       <c r="H37">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J37">
-        <v>2008.41</v>
+        <v>5098.41</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2613,28 +2739,28 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="E38" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="F38" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
       <c r="G38" t="s">
-        <v>336</v>
+        <v>369</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J38">
-        <v>19851.56</v>
+        <v>5012.96</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2645,28 +2771,28 @@
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="E39" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="F39" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="G39" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I39">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J39">
-        <v>17974.88</v>
+        <v>4593.46</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2677,28 +2803,28 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E40" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="F40" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="G40" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I40">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J40">
-        <v>12471.99</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2709,28 +2835,28 @@
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="F41" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="G41" t="s">
-        <v>336</v>
+        <v>371</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I41">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J41">
-        <v>12018.88</v>
+        <v>12108.37</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2741,28 +2867,28 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="E42" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F42" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="G42" t="s">
-        <v>336</v>
+        <v>372</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J42">
-        <v>5095.76</v>
+        <v>29957.98</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2773,28 +2899,28 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="E43" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="F43" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="G43" t="s">
-        <v>337</v>
+        <v>372</v>
       </c>
       <c r="H43">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J43">
-        <v>5035</v>
+        <v>27165</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2805,28 +2931,28 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D44" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E44" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="F44" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="G44" t="s">
-        <v>336</v>
+        <v>372</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J44">
-        <v>4798.89</v>
+        <v>18145.98</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2837,28 +2963,28 @@
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E45" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="F45" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="G45" t="s">
-        <v>336</v>
+        <v>373</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I45">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J45">
-        <v>4023.52</v>
+        <v>13066.8</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2869,28 +2995,28 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E46" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="F46" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="G46" t="s">
-        <v>337</v>
+        <v>373</v>
       </c>
       <c r="H46">
         <v>30</v>
       </c>
       <c r="I46">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J46">
-        <v>3224</v>
+        <v>11947.81</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2901,28 +3027,28 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="E47" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="F47" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="G47" t="s">
-        <v>338</v>
+        <v>372</v>
       </c>
       <c r="H47">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J47">
-        <v>6909.08</v>
+        <v>11750</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2933,28 +3059,28 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E48" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="F48" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="G48" t="s">
-        <v>338</v>
+        <v>372</v>
       </c>
       <c r="H48">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J48">
-        <v>5428.19</v>
+        <v>9970.299999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2965,28 +3091,28 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E49" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="F49" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="G49" t="s">
-        <v>339</v>
+        <v>374</v>
       </c>
       <c r="H49">
         <v>30</v>
       </c>
       <c r="I49">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J49">
-        <v>12094.19</v>
+        <v>2276.1</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2997,28 +3123,28 @@
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="E50" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="F50" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="G50" t="s">
-        <v>340</v>
+        <v>374</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I50">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J50">
-        <v>10045.19</v>
+        <v>1861.92</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -3029,28 +3155,28 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D51" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="E51" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="F51" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="G51" t="s">
-        <v>339</v>
+        <v>374</v>
       </c>
       <c r="H51">
         <v>30</v>
       </c>
       <c r="I51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J51">
-        <v>5746.02</v>
+        <v>1097.71</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -3061,28 +3187,28 @@
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="E52" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="F52" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="G52" t="s">
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="H52">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I52">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J52">
-        <v>4102.8</v>
+        <v>20013.86</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3093,28 +3219,28 @@
         <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D53" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="E53" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="F53" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="G53" t="s">
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="H53">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J53">
-        <v>4012.03</v>
+        <v>16564.46</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3125,28 +3251,28 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D54" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="E54" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="F54" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="G54" t="s">
-        <v>341</v>
+        <v>375</v>
       </c>
       <c r="H54">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I54">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J54">
-        <v>4957.22</v>
+        <v>12102.26</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3157,28 +3283,28 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="E55" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F55" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="G55" t="s">
-        <v>341</v>
+        <v>376</v>
       </c>
       <c r="H55">
         <v>30</v>
       </c>
       <c r="I55">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J55">
-        <v>3018.59</v>
+        <v>7128.02</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -3189,28 +3315,28 @@
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="E56" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F56" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="G56" t="s">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J56">
-        <v>18854</v>
+        <v>20058.04</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3218,31 +3344,31 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="D57" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="E57" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="F57" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
       <c r="G57" t="s">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="H57">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I57">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J57">
-        <v>16969.68</v>
+        <v>15059.09</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3250,31 +3376,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="F58" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="G58" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
       <c r="H58">
         <v>30</v>
       </c>
       <c r="I58">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J58">
-        <v>14982.92</v>
+        <v>10006.6</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3282,31 +3408,31 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="E59" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="F59" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
       <c r="G59" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
       <c r="H59">
         <v>30</v>
       </c>
       <c r="I59">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J59">
-        <v>12114.13</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3314,31 +3440,31 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D60" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="E60" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="F60" t="s">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="G60" t="s">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="H60">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I60">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J60">
-        <v>12026.99</v>
+        <v>9966.129999999999</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3346,31 +3472,31 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="E61" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F61" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="G61" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
       <c r="H61">
         <v>30</v>
       </c>
       <c r="I61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J61">
-        <v>8169.29</v>
+        <v>7499.65</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3378,31 +3504,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E62" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="F62" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="G62" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
       <c r="H62">
         <v>30</v>
       </c>
       <c r="I62">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J62">
-        <v>4193.74</v>
+        <v>569.76</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3410,31 +3536,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D63" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E63" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="F63" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="G63" t="s">
-        <v>343</v>
+        <v>379</v>
       </c>
       <c r="H63">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J63">
-        <v>3559.13</v>
+        <v>30026.79</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3442,31 +3568,31 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="E64" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="F64" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="G64" t="s">
-        <v>343</v>
+        <v>379</v>
       </c>
       <c r="H64">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J64">
-        <v>3062.51</v>
+        <v>29600.3</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3474,31 +3600,31 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="E65" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="F65" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="G65" t="s">
-        <v>343</v>
+        <v>379</v>
       </c>
       <c r="H65">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J65">
-        <v>3009.54</v>
+        <v>12092.62</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3506,31 +3632,31 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D66" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="E66" t="s">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="F66" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="G66" t="s">
-        <v>343</v>
+        <v>380</v>
       </c>
       <c r="H66">
         <v>30</v>
       </c>
       <c r="I66">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J66">
-        <v>938.27</v>
+        <v>5047.58</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3538,31 +3664,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D67" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E67" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="F67" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="G67" t="s">
-        <v>344</v>
+        <v>381</v>
       </c>
       <c r="H67">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J67">
-        <v>19977.54</v>
+        <v>20041.35</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3570,31 +3696,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D68" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="E68" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F68" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="G68" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="H68">
         <v>30</v>
       </c>
       <c r="I68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J68">
-        <v>15468.68</v>
+        <v>19743.38</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3602,31 +3728,31 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
       <c r="E69" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="F69" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="G69" t="s">
-        <v>344</v>
+        <v>382</v>
       </c>
       <c r="H69">
         <v>30</v>
       </c>
       <c r="I69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J69">
-        <v>7052.84</v>
+        <v>19968.87</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3634,31 +3760,31 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D70" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="E70" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F70" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
       <c r="G70" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="H70">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J70">
-        <v>5113.17</v>
+        <v>11808.51</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3666,31 +3792,31 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D71" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E71" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="F71" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="G71" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="H71">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J71">
-        <v>5060.89</v>
+        <v>11317.8</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3698,31 +3824,31 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C72" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D72" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E72" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="F72" t="s">
-        <v>322</v>
+        <v>341</v>
       </c>
       <c r="G72" t="s">
-        <v>344</v>
+        <v>382</v>
       </c>
       <c r="H72">
         <v>30</v>
       </c>
       <c r="I72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J72">
-        <v>4971.65</v>
+        <v>9906.799999999999</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3730,31 +3856,319 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C73" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="E73" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="F73" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="G73" t="s">
-        <v>344</v>
+        <v>382</v>
       </c>
       <c r="H73">
         <v>30</v>
       </c>
       <c r="I73">
+        <v>3</v>
+      </c>
+      <c r="J73">
+        <v>9829.65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74" t="s">
+        <v>165</v>
+      </c>
+      <c r="E74" t="s">
+        <v>241</v>
+      </c>
+      <c r="F74" t="s">
+        <v>343</v>
+      </c>
+      <c r="G74" t="s">
+        <v>384</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74">
+        <v>30220.79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" t="s">
+        <v>90</v>
+      </c>
+      <c r="D75" t="s">
+        <v>166</v>
+      </c>
+      <c r="E75" t="s">
+        <v>242</v>
+      </c>
+      <c r="F75" t="s">
+        <v>344</v>
+      </c>
+      <c r="G75" t="s">
+        <v>384</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+      <c r="J75">
+        <v>19993.39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" t="s">
+        <v>233</v>
+      </c>
+      <c r="E76" t="s">
+        <v>266</v>
+      </c>
+      <c r="F76" t="s">
+        <v>345</v>
+      </c>
+      <c r="G76" t="s">
+        <v>385</v>
+      </c>
+      <c r="H76">
+        <v>30</v>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76">
+        <v>11983.27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>42</v>
+      </c>
+      <c r="C77" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77" t="s">
+        <v>195</v>
+      </c>
+      <c r="E77" t="s">
+        <v>246</v>
+      </c>
+      <c r="F77" t="s">
+        <v>346</v>
+      </c>
+      <c r="G77" t="s">
+        <v>384</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>2</v>
+      </c>
+      <c r="J77">
+        <v>9970.799999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" t="s">
+        <v>234</v>
+      </c>
+      <c r="E78" t="s">
+        <v>238</v>
+      </c>
+      <c r="F78" t="s">
+        <v>347</v>
+      </c>
+      <c r="G78" t="s">
+        <v>385</v>
+      </c>
+      <c r="H78">
+        <v>30</v>
+      </c>
+      <c r="I78">
+        <v>2</v>
+      </c>
+      <c r="J78">
+        <v>3203.76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" t="s">
+        <v>158</v>
+      </c>
+      <c r="D79" t="s">
+        <v>235</v>
+      </c>
+      <c r="E79" t="s">
+        <v>270</v>
+      </c>
+      <c r="F79" t="s">
+        <v>348</v>
+      </c>
+      <c r="G79" t="s">
+        <v>386</v>
+      </c>
+      <c r="H79">
+        <v>30</v>
+      </c>
+      <c r="I79">
         <v>1</v>
       </c>
-      <c r="J73">
-        <v>3000.94</v>
+      <c r="J79">
+        <v>16614.84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" t="s">
+        <v>159</v>
+      </c>
+      <c r="D80" t="s">
+        <v>236</v>
+      </c>
+      <c r="E80" t="s">
+        <v>245</v>
+      </c>
+      <c r="F80" t="s">
+        <v>349</v>
+      </c>
+      <c r="G80" t="s">
+        <v>386</v>
+      </c>
+      <c r="H80">
+        <v>30</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>12009.69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" t="s">
+        <v>160</v>
+      </c>
+      <c r="D81" t="s">
+        <v>221</v>
+      </c>
+      <c r="E81" t="s">
+        <v>259</v>
+      </c>
+      <c r="F81" t="s">
+        <v>350</v>
+      </c>
+      <c r="G81" t="s">
+        <v>386</v>
+      </c>
+      <c r="H81">
+        <v>30</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>9900.129999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" t="s">
+        <v>237</v>
+      </c>
+      <c r="E82" t="s">
+        <v>261</v>
+      </c>
+      <c r="F82" t="s">
+        <v>351</v>
+      </c>
+      <c r="G82" t="s">
+        <v>386</v>
+      </c>
+      <c r="H82">
+        <v>30</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>8081.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>